<commit_message>
TCID 9,10,11 (Pass) -- Vat number does not reflect in SAP*
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupUpdated.xlsx
+++ b/src/test/resources/data/jdgroupUpdated.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8663151-4375-4DBD-A187-67BEA7BEE250}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6AAFF6-0504-485A-8DBE-F800BD1A9FE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3510" yWindow="-10910" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3510" yWindow="-10910" windowWidth="19420" windowHeight="10420" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2545" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2545" uniqueCount="633">
   <si>
     <t>testSuitID</t>
   </si>
@@ -2028,6 +2028,12 @@
   </si>
   <si>
     <t>5311ASSA32</t>
+  </si>
+  <si>
+    <t>8304153864085</t>
+  </si>
+  <si>
+    <t>BackendLastName</t>
   </si>
 </sst>
 </file>
@@ -3271,10 +3277,10 @@
   <dimension ref="A1:R55"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -3445,7 +3451,7 @@
         <v>119</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F4" s="50" t="s">
         <v>507</v>
@@ -3685,7 +3691,7 @@
         <v>220</v>
       </c>
       <c r="E10" s="50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="51" t="s">
         <v>199</v>
@@ -6677,12 +6683,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H2" sqref="H2"/>
       <selection pane="topRight" activeCell="H2" sqref="H2"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -6828,7 +6834,7 @@
       </c>
       <c r="H2" s="18"/>
       <c r="I2" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J2" s="18"/>
       <c r="K2" s="18" t="s">
@@ -8259,7 +8265,7 @@
       <selection activeCell="H2" sqref="H2"/>
       <selection pane="topRight" activeCell="H2" sqref="H2"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -11371,7 +11377,7 @@
       <selection activeCell="H2" sqref="H2"/>
       <selection pane="topRight" activeCell="H2" sqref="H2"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -13559,7 +13565,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -13907,7 +13913,7 @@
         <v>610</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>611</v>
+        <v>632</v>
       </c>
       <c r="F10" s="21" t="s">
         <v>126</v>
@@ -13916,7 +13922,7 @@
         <v>129</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>612</v>
+        <v>631</v>
       </c>
       <c r="I10" s="28" t="s">
         <v>627</v>
@@ -15697,7 +15703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD40FD6A-3206-4F33-9099-D76F7461AC19}">
   <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -16693,6 +16699,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16841,25 +16865,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16876,29 +16907,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update to include 2 test methods
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupUpdated.xlsx
+++ b/src/test/resources/data/jdgroupUpdated.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6AAFF6-0504-485A-8DBE-F800BD1A9FE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3510" yWindow="-10910" windowWidth="19420" windowHeight="10420" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3510" yWindow="-10905" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -60,12 +59,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1100-000001000000}">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -82,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1100-000002000000}">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -104,12 +103,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1800-000001000000}">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2039,7 +2038,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -2135,7 +2134,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2157,6 +2156,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2205,7 +2210,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2391,13 +2396,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="4"/>
+    <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
   <dxfs count="54">
     <dxf>
@@ -2996,7 +3004,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3029,26 +3037,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3081,23 +3072,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3273,33 +3247,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R55"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomRight" activeCell="A54" sqref="A54:XFD54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" style="58" customWidth="1"/>
-    <col min="2" max="2" width="93.54296875" style="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" style="58" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="90.7265625" style="58" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" style="58" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" style="58" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="33.7265625" style="58" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.81640625" style="58" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.453125" style="58" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.7265625" style="58" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.453125" style="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="27.1796875" style="58" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="31.453125" style="58" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.81640625" style="58" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.1796875" style="58"/>
+    <col min="2" max="2" width="93.5703125" style="58" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="58" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="90.7109375" style="58" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="58" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="58" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" style="58" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" style="58" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.42578125" style="58" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.7109375" style="58" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" style="58" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="27.140625" style="58" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="31.42578125" style="58" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" style="58" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -3355,8 +3329,8 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="29">
-      <c r="A2" s="50">
+    <row r="2" spans="1:17" ht="30">
+      <c r="A2" s="79">
         <v>1</v>
       </c>
       <c r="B2" s="50" t="s">
@@ -3369,7 +3343,7 @@
         <v>121</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="50" t="s">
         <v>507</v>
@@ -3396,8 +3370,8 @@
       <c r="P2" s="50"/>
       <c r="Q2" s="50"/>
     </row>
-    <row r="3" spans="1:17" ht="29">
-      <c r="A3" s="50">
+    <row r="3" spans="1:17" ht="30">
+      <c r="A3" s="79">
         <v>2</v>
       </c>
       <c r="B3" s="50" t="s">
@@ -3410,7 +3384,7 @@
         <v>120</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="50" t="s">
         <v>507</v>
@@ -3437,8 +3411,8 @@
       <c r="P3" s="50"/>
       <c r="Q3" s="50"/>
     </row>
-    <row r="4" spans="1:17" ht="29">
-      <c r="A4" s="50">
+    <row r="4" spans="1:17" ht="30">
+      <c r="A4" s="79">
         <v>3</v>
       </c>
       <c r="B4" s="50" t="s">
@@ -3451,7 +3425,7 @@
         <v>119</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="50" t="s">
         <v>507</v>
@@ -3478,8 +3452,8 @@
       <c r="P4" s="50"/>
       <c r="Q4" s="50"/>
     </row>
-    <row r="5" spans="1:17" ht="29">
-      <c r="A5" s="50">
+    <row r="5" spans="1:17" ht="30">
+      <c r="A5" s="79">
         <v>4</v>
       </c>
       <c r="B5" s="50" t="s">
@@ -3492,7 +3466,7 @@
         <v>118</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="50" t="s">
         <v>507</v>
@@ -3519,8 +3493,8 @@
       <c r="P5" s="50"/>
       <c r="Q5" s="50"/>
     </row>
-    <row r="6" spans="1:17" ht="29">
-      <c r="A6" s="50">
+    <row r="6" spans="1:17" ht="30">
+      <c r="A6" s="79">
         <v>5</v>
       </c>
       <c r="B6" s="50" t="s">
@@ -3533,7 +3507,7 @@
         <v>125</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="50" t="s">
         <v>507</v>
@@ -3560,7 +3534,7 @@
       <c r="P6" s="50"/>
       <c r="Q6" s="50"/>
     </row>
-    <row r="7" spans="1:17" ht="29">
+    <row r="7" spans="1:17" ht="30">
       <c r="A7" s="50">
         <v>6</v>
       </c>
@@ -3599,7 +3573,7 @@
       <c r="P7" s="50"/>
       <c r="Q7" s="50"/>
     </row>
-    <row r="8" spans="1:17" ht="29">
+    <row r="8" spans="1:17" ht="30">
       <c r="A8" s="50">
         <v>7</v>
       </c>
@@ -3638,7 +3612,7 @@
       <c r="P8" s="50"/>
       <c r="Q8" s="50"/>
     </row>
-    <row r="9" spans="1:17" ht="29">
+    <row r="9" spans="1:17" ht="30">
       <c r="A9" s="50">
         <v>8</v>
       </c>
@@ -3677,8 +3651,8 @@
       <c r="P9" s="50"/>
       <c r="Q9" s="50"/>
     </row>
-    <row r="10" spans="1:17" ht="29">
-      <c r="A10" s="50">
+    <row r="10" spans="1:17" ht="30">
+      <c r="A10" s="79">
         <v>9</v>
       </c>
       <c r="B10" s="50" t="s">
@@ -3716,8 +3690,8 @@
       <c r="P10" s="50"/>
       <c r="Q10" s="50"/>
     </row>
-    <row r="11" spans="1:17" ht="29">
-      <c r="A11" s="50">
+    <row r="11" spans="1:17" ht="30">
+      <c r="A11" s="79">
         <v>10</v>
       </c>
       <c r="B11" s="50" t="s">
@@ -3730,7 +3704,7 @@
         <v>221</v>
       </c>
       <c r="E11" s="50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="51" t="s">
         <v>199</v>
@@ -3755,8 +3729,8 @@
       <c r="P11" s="50"/>
       <c r="Q11" s="50"/>
     </row>
-    <row r="12" spans="1:17" ht="29">
-      <c r="A12" s="50">
+    <row r="12" spans="1:17" ht="30">
+      <c r="A12" s="79">
         <v>11</v>
       </c>
       <c r="B12" s="50" t="s">
@@ -3769,7 +3743,7 @@
         <v>222</v>
       </c>
       <c r="E12" s="50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="51" t="s">
         <v>199</v>
@@ -3794,7 +3768,7 @@
       <c r="P12" s="50"/>
       <c r="Q12" s="50"/>
     </row>
-    <row r="13" spans="1:17" ht="29">
+    <row r="13" spans="1:17" ht="30">
       <c r="A13" s="50">
         <v>12</v>
       </c>
@@ -3833,7 +3807,7 @@
       <c r="P13" s="50"/>
       <c r="Q13" s="50"/>
     </row>
-    <row r="14" spans="1:17" ht="29">
+    <row r="14" spans="1:17" ht="30">
       <c r="A14" s="50">
         <v>13</v>
       </c>
@@ -3872,7 +3846,7 @@
       <c r="P14" s="50"/>
       <c r="Q14" s="50"/>
     </row>
-    <row r="15" spans="1:17" ht="29">
+    <row r="15" spans="1:17" ht="30">
       <c r="A15" s="50">
         <v>14</v>
       </c>
@@ -3911,7 +3885,7 @@
       <c r="P15" s="50"/>
       <c r="Q15" s="50"/>
     </row>
-    <row r="16" spans="1:17" ht="29">
+    <row r="16" spans="1:17" ht="30">
       <c r="A16" s="50">
         <v>15</v>
       </c>
@@ -3952,7 +3926,7 @@
       <c r="P16" s="50"/>
       <c r="Q16" s="50"/>
     </row>
-    <row r="17" spans="1:18" ht="29">
+    <row r="17" spans="1:18" ht="30">
       <c r="A17" s="50">
         <v>16</v>
       </c>
@@ -3993,7 +3967,7 @@
       <c r="P17" s="50"/>
       <c r="Q17" s="50"/>
     </row>
-    <row r="18" spans="1:18" ht="29">
+    <row r="18" spans="1:18" ht="30">
       <c r="A18" s="50">
         <v>17</v>
       </c>
@@ -4034,7 +4008,7 @@
       <c r="P18" s="50"/>
       <c r="Q18" s="50"/>
     </row>
-    <row r="19" spans="1:18" ht="29">
+    <row r="19" spans="1:18" ht="30">
       <c r="A19" s="50">
         <v>18</v>
       </c>
@@ -4075,7 +4049,7 @@
       <c r="P19" s="50"/>
       <c r="Q19" s="50"/>
     </row>
-    <row r="20" spans="1:18" ht="29">
+    <row r="20" spans="1:18" ht="30">
       <c r="A20" s="50">
         <v>19</v>
       </c>
@@ -4116,7 +4090,7 @@
       <c r="P20" s="50"/>
       <c r="Q20" s="50"/>
     </row>
-    <row r="21" spans="1:18" ht="29">
+    <row r="21" spans="1:18" ht="30">
       <c r="A21" s="50">
         <v>20</v>
       </c>
@@ -4535,7 +4509,7 @@
       <c r="O31" s="50"/>
       <c r="P31" s="50"/>
     </row>
-    <row r="32" spans="1:18" ht="29">
+    <row r="32" spans="1:18" ht="30">
       <c r="A32" s="50">
         <v>31</v>
       </c>
@@ -5418,195 +5392,195 @@
     <cfRule type="duplicateValues" dxfId="47" priority="12"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-000009000000}"/>
-    <hyperlink ref="K3" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0700-00000A000000}"/>
-    <hyperlink ref="G3" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0700-00000B000000}"/>
-    <hyperlink ref="H4" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-00000C000000}"/>
-    <hyperlink ref="K4" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0700-00000D000000}"/>
-    <hyperlink ref="G4" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0700-00000E000000}"/>
-    <hyperlink ref="H5" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-00000F000000}"/>
-    <hyperlink ref="K5" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0700-000010000000}"/>
-    <hyperlink ref="G5" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0700-000011000000}"/>
-    <hyperlink ref="H6" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-000012000000}"/>
-    <hyperlink ref="K6" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0700-000013000000}"/>
-    <hyperlink ref="G6" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0700-000014000000}"/>
-    <hyperlink ref="G7" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-000015000000}"/>
-    <hyperlink ref="G8:G9" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-000016000000}"/>
-    <hyperlink ref="H7" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend" xr:uid="{00000000-0004-0000-0700-000017000000}"/>
-    <hyperlink ref="H8:H9" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend" xr:uid="{00000000-0004-0000-0700-000018000000}"/>
-    <hyperlink ref="J8:J9" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0700-000019000000}"/>
-    <hyperlink ref="J7" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0700-00001A000000}"/>
-    <hyperlink ref="G2" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0700-00001B000000}"/>
-    <hyperlink ref="H2" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-00001C000000}"/>
-    <hyperlink ref="G10:G14" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-00001E000000}"/>
-    <hyperlink ref="H10" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0700-00001F000000}"/>
-    <hyperlink ref="H11:H14" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0700-000020000000}"/>
-    <hyperlink ref="G15" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-000021000000}"/>
-    <hyperlink ref="H15" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0700-000022000000}"/>
-    <hyperlink ref="G16" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0700-000023000000}"/>
-    <hyperlink ref="H16" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0700-000024000000}"/>
-    <hyperlink ref="I16" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-000025000000}"/>
-    <hyperlink ref="G17" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0700-000026000000}"/>
-    <hyperlink ref="G18" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0700-000027000000}"/>
-    <hyperlink ref="G19" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0700-000028000000}"/>
-    <hyperlink ref="G20" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0700-000029000000}"/>
-    <hyperlink ref="H17" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0700-00002A000000}"/>
-    <hyperlink ref="H18" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0700-00002B000000}"/>
-    <hyperlink ref="H19" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0700-00002C000000}"/>
-    <hyperlink ref="H20" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0700-00002D000000}"/>
-    <hyperlink ref="I17" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-00002E000000}"/>
-    <hyperlink ref="I18" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-00002F000000}"/>
-    <hyperlink ref="I19" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-000030000000}"/>
-    <hyperlink ref="I20" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-000031000000}"/>
-    <hyperlink ref="G21" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0700-000032000000}"/>
-    <hyperlink ref="H21" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0700-000033000000}"/>
-    <hyperlink ref="I21" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-000034000000}"/>
-    <hyperlink ref="G27" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0700-000035000000}"/>
-    <hyperlink ref="H27" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0700-000036000000}"/>
-    <hyperlink ref="L27" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-000037000000}"/>
-    <hyperlink ref="N27" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0700-000038000000}"/>
-    <hyperlink ref="G24" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0700-000039000000}"/>
-    <hyperlink ref="G25" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0700-00003A000000}"/>
-    <hyperlink ref="G22" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0700-00003B000000}"/>
-    <hyperlink ref="G23" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0700-00003C000000}"/>
-    <hyperlink ref="G26" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0700-00003D000000}"/>
-    <hyperlink ref="J10:J15" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0700-00003E000000}"/>
-    <hyperlink ref="K17:K21" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0700-00003F000000}"/>
-    <hyperlink ref="K16" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0700-000040000000}"/>
-    <hyperlink ref="I27" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0700-000041000000}"/>
-    <hyperlink ref="J27" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0700-000042000000}"/>
-    <hyperlink ref="M27" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0700-000043000000}"/>
-    <hyperlink ref="K27" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0700-000044000000}"/>
-    <hyperlink ref="O27" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0700-000045000000}"/>
-    <hyperlink ref="G28" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0700-000046000000}"/>
-    <hyperlink ref="G30" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0700-000047000000}"/>
-    <hyperlink ref="H28" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0700-000048000000}"/>
-    <hyperlink ref="H30" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0700-000049000000}"/>
-    <hyperlink ref="L28" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-00004A000000}"/>
-    <hyperlink ref="L30" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-00004B000000}"/>
-    <hyperlink ref="N28" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0700-00004C000000}"/>
-    <hyperlink ref="N30" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0700-00004D000000}"/>
-    <hyperlink ref="I28" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0700-00004E000000}"/>
-    <hyperlink ref="I30" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0700-00004F000000}"/>
-    <hyperlink ref="J28" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0700-000050000000}"/>
-    <hyperlink ref="J30" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0700-000051000000}"/>
-    <hyperlink ref="M28" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0700-000052000000}"/>
-    <hyperlink ref="M30" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0700-000053000000}"/>
-    <hyperlink ref="K28" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0700-000054000000}"/>
-    <hyperlink ref="K30" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0700-000055000000}"/>
-    <hyperlink ref="O28" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0700-000056000000}"/>
-    <hyperlink ref="O30" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0700-000057000000}"/>
-    <hyperlink ref="G31" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0700-000058000000}"/>
-    <hyperlink ref="H31" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0700-000059000000}"/>
-    <hyperlink ref="K31" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-00005A000000}"/>
-    <hyperlink ref="M31" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0700-00005B000000}"/>
-    <hyperlink ref="I31" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0700-00005C000000}"/>
-    <hyperlink ref="L31" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0700-00005D000000}"/>
-    <hyperlink ref="J31" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0700-00005E000000}"/>
-    <hyperlink ref="N31" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0700-00005F000000}"/>
-    <hyperlink ref="G29" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0700-000060000000}"/>
-    <hyperlink ref="H29" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0700-000061000000}"/>
-    <hyperlink ref="L29" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-000062000000}"/>
-    <hyperlink ref="N29" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0700-000063000000}"/>
-    <hyperlink ref="I29" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0700-000064000000}"/>
-    <hyperlink ref="J29" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0700-000065000000}"/>
-    <hyperlink ref="M29" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0700-000066000000}"/>
-    <hyperlink ref="K29" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0700-000067000000}"/>
-    <hyperlink ref="O29" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0700-000068000000}"/>
-    <hyperlink ref="G32" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0700-000069000000}"/>
-    <hyperlink ref="H32" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0700-00006A000000}"/>
-    <hyperlink ref="L32" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-00006B000000}"/>
-    <hyperlink ref="I32" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0700-00006D000000}"/>
-    <hyperlink ref="J32" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0700-00006E000000}"/>
-    <hyperlink ref="M32" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0700-00006F000000}"/>
-    <hyperlink ref="K32" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0700-000070000000}"/>
-    <hyperlink ref="Q32" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0700-000071000000}"/>
-    <hyperlink ref="R32" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0700-000072000000}"/>
-    <hyperlink ref="G34" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0700-000073000000}"/>
-    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0700-000074000000}"/>
-    <hyperlink ref="H37" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0700-000075000000}"/>
-    <hyperlink ref="H33" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0700-000076000000}"/>
-    <hyperlink ref="I33" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0700-000077000000}"/>
-    <hyperlink ref="J33" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0700-000078000000}"/>
-    <hyperlink ref="K33" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-000079000000}"/>
-    <hyperlink ref="L33" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0700-00007A000000}"/>
-    <hyperlink ref="M33" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0700-00007B000000}"/>
-    <hyperlink ref="N33" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0700-00007C000000}"/>
-    <hyperlink ref="G33" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase" xr:uid="{00000000-0004-0000-0700-00007D000000}"/>
-    <hyperlink ref="H34" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase" xr:uid="{00000000-0004-0000-0700-00007E000000}"/>
-    <hyperlink ref="J34" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0700-00007F000000}"/>
-    <hyperlink ref="K34" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0700-000080000000}"/>
-    <hyperlink ref="L34" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-000081000000}"/>
-    <hyperlink ref="M34" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0700-000082000000}"/>
-    <hyperlink ref="N34" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0700-000083000000}"/>
-    <hyperlink ref="O34" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0700-000084000000}"/>
-    <hyperlink ref="M35" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0700-000085000000}"/>
-    <hyperlink ref="H47" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails" xr:uid="{00000000-0004-0000-0700-000086000000}"/>
-    <hyperlink ref="H48" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails" xr:uid="{00000000-0004-0000-0700-000087000000}"/>
-    <hyperlink ref="I47" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor" xr:uid="{00000000-0004-0000-0700-000088000000}"/>
-    <hyperlink ref="I48" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor" xr:uid="{00000000-0004-0000-0700-000089000000}"/>
-    <hyperlink ref="J47" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails" xr:uid="{00000000-0004-0000-0700-00008A000000}"/>
-    <hyperlink ref="J48" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails" xr:uid="{00000000-0004-0000-0700-00008B000000}"/>
-    <hyperlink ref="G47" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0700-000090000000}"/>
-    <hyperlink ref="G48" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0700-000091000000}"/>
-    <hyperlink ref="G49" location="'ic_SubscribeNews_DupliEmailID++'!A1" display="ic_SubscribeNews_DupliEmailID" xr:uid="{00000000-0004-0000-0700-000092000000}"/>
-    <hyperlink ref="I40" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0700-000095000000}"/>
-    <hyperlink ref="G40" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0700-000096000000}"/>
-    <hyperlink ref="H41" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0700-000097000000}"/>
-    <hyperlink ref="J40" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0700-000098000000}"/>
-    <hyperlink ref="K40" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0700-000099000000}"/>
-    <hyperlink ref="L40" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0700-00009A000000}"/>
-    <hyperlink ref="M40" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0700-00009B000000}"/>
-    <hyperlink ref="N40" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0700-00009C000000}"/>
-    <hyperlink ref="Q40" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0700-00009E000000}"/>
-    <hyperlink ref="G41:G42" location="'ic_login++'!A1" display="ic_login" xr:uid="{97F84805-E581-459E-A6FB-8A4EB0A5E7ED}"/>
-    <hyperlink ref="I41:I42" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{60A7E164-E4F7-44DA-8690-84942310E0BB}"/>
-    <hyperlink ref="H40:H42" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{417BB145-5C27-4678-8A4E-BDE7A773BCDD}"/>
-    <hyperlink ref="J40:J42" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{9F8D8FA3-7C9E-43E0-8EE9-C6217AF49C09}"/>
-    <hyperlink ref="K40:K42" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{B4C7E1AE-FAFD-415F-B821-F94BF8170858}"/>
-    <hyperlink ref="L40:L42" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{3BDF9676-068B-4A3D-852D-C16989CE97B9}"/>
-    <hyperlink ref="M40:M42" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{0A59B855-2797-4809-9E4C-9F90E6C86759}"/>
-    <hyperlink ref="N40:N42" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{5A2BABEF-B434-46AA-AFA2-FFB35868DC50}"/>
-    <hyperlink ref="Q40:Q42" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{CBDB1D9C-7728-494A-A0B1-1C7BE9D3E45D}"/>
-    <hyperlink ref="H54" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{37966542-A73F-4D1F-B63E-3B436D0DAF4A}"/>
-    <hyperlink ref="M47" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{7C5CED48-AE56-4969-BEBC-B5B3A8E275CC}"/>
-    <hyperlink ref="N47" location="'CreditApp_NavigateFilter++'!A1" display="CreditApp_NavigateFilter" xr:uid="{345B6C5E-45C4-4F91-A79A-19E3982C8C92}"/>
-    <hyperlink ref="O47" location="'CreditStatusVerification++'!A1" display="CreditStatusVerification" xr:uid="{016B4CD4-C812-4232-BA07-819DD85E9DF9}"/>
-    <hyperlink ref="N32" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0700-00006C000000}"/>
-    <hyperlink ref="J2" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{41A192C1-C805-44EA-A5B1-D5BFEDEE0CA8}"/>
-    <hyperlink ref="J16:J21" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{E117577A-CEDC-4A1C-88A3-6B50A0AB895E}"/>
-    <hyperlink ref="P32" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{AE5A2668-9089-474A-8EDC-8C5E743A4780}"/>
-    <hyperlink ref="P40:P42" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{DEC89986-4AC0-45D7-81DD-64BB1C3C9DA9}"/>
-    <hyperlink ref="L48" location="'EnterContact++'!A1" display="EnterContact" xr:uid="{00000000-0004-0000-0700-00008F000000}"/>
-    <hyperlink ref="L47" location="'EnterContact++'!A1" display="EnterContact" xr:uid="{00000000-0004-0000-0700-00008E000000}"/>
-    <hyperlink ref="K48" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails" xr:uid="{00000000-0004-0000-0700-00008D000000}"/>
-    <hyperlink ref="K47" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails" xr:uid="{00000000-0004-0000-0700-00008C000000}"/>
-    <hyperlink ref="G39" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{24E2DB2C-8752-416C-8E5E-D387B78964B0}"/>
-    <hyperlink ref="G38" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{FBD7087C-EA59-4AD8-9DB8-D18431202AFB}"/>
-    <hyperlink ref="G53:G54" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{D06EF77D-6C78-48CF-9BB8-E0E328BED80E}"/>
-    <hyperlink ref="H53" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{958205DD-4660-453E-BD5F-DA6DA394D1BD}"/>
-    <hyperlink ref="I54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{AF4EA3C4-5F76-4737-B165-C048C8D91BCE}"/>
-    <hyperlink ref="I53" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{7A911EB4-8750-446D-9BE3-671BCBEB4CDE}"/>
-    <hyperlink ref="J54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{8252C90A-3611-4069-B00D-7A1E40F13851}"/>
-    <hyperlink ref="G35" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase" xr:uid="{F7F02630-F71F-429E-840E-4E5229C8B760}"/>
-    <hyperlink ref="H35" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{665E8536-7F52-4F37-A9FF-C4A5E309086C}"/>
-    <hyperlink ref="I35" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{E3550F14-1831-4956-BBB4-8A7AC7A59598}"/>
-    <hyperlink ref="J35" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{D330C808-580A-4C9E-8767-67F7D09FCD87}"/>
-    <hyperlink ref="K35" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{59F29986-395D-4977-9E6B-2D53BAC6E048}"/>
-    <hyperlink ref="L35" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{05971A25-0B9A-46E4-ABD5-B0C3E785FC82}"/>
-    <hyperlink ref="G36" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{6192C788-E436-4D10-81FB-57F48F1F86F1}"/>
-    <hyperlink ref="H36" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard" xr:uid="{7674EF96-12B2-436D-BC0E-E4D444C5BD82}"/>
-    <hyperlink ref="I36" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{BCA1C8F1-5517-40E2-B47A-69A469F05EF4}"/>
-    <hyperlink ref="J36" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{C678C2E8-5C97-4989-9B69-DEADB76AE315}"/>
-    <hyperlink ref="K37" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{25CB71F0-8283-4453-B74A-88F1F972AB17}"/>
-    <hyperlink ref="I37" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard" xr:uid="{7FB423EB-FF4B-4278-8912-EA5D8C66B7F9}"/>
-    <hyperlink ref="K36" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{F3DA866D-7667-4B1A-B74A-BFE9EEF1A691}"/>
-    <hyperlink ref="L37" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{6B95C44A-F62A-4C5C-96BA-68B9E583839F}"/>
-    <hyperlink ref="H38" location="'giftCardReport++'!A1" display="giftCardReport" xr:uid="{9B3B1D17-E2A3-4F93-98ED-2DC98451EA60}"/>
-    <hyperlink ref="H39" location="'giftCardReport++'!A1" display="giftCardReport" xr:uid="{484E64EB-A874-4088-A91D-D338A7A6E071}"/>
-    <hyperlink ref="G50" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy" xr:uid="{CE85C0C1-7977-4974-9826-B84E919F734C}"/>
-    <hyperlink ref="G50:G52" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy" xr:uid="{E626E1CA-789A-4FC5-80C4-3220719E8CB8}"/>
-    <hyperlink ref="J3:J6" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{E9949BB0-990F-410C-9C18-8F9FCDC01289}"/>
+    <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="K3" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G3" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H4" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="K4" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G4" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H5" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="K5" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G5" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H6" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="K6" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G6" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="G7" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G8:G9" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H7" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend"/>
+    <hyperlink ref="H8:H9" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend"/>
+    <hyperlink ref="J8:J9" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="J7" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G2" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H2" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G10:G14" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H10" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
+    <hyperlink ref="H11:H14" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
+    <hyperlink ref="G15" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H15" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
+    <hyperlink ref="G16" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H16" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="I16" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G17" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G18" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G19" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G20" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H17" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="H18" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="H19" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="H20" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="I17" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I18" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I19" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I20" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G21" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H21" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="I21" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G27" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H27" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L27" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N27" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="G24" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="G25" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="G22" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="G23" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="G26" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="J10:J15" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="K17:K21" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="K16" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="I27" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J27" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="M27" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="K27" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="O27" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="G28" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G30" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H28" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="H30" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L28" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="L30" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N28" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="N30" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="I28" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="I30" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J28" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="J30" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="M28" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="M30" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="K28" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="K30" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="O28" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="O30" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="G31" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H31" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="K31" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="M31" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="I31" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="L31" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="J31" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="N31" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="G29" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H29" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L29" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N29" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="I29" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J29" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="M29" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="K29" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="O29" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="G32" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H32" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L32" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I32" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J32" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="M32" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="K32" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="Q32" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="R32" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G34" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H37" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H33" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="I33" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J33" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="K33" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="L33" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="M33" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="N33" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="G33" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
+    <hyperlink ref="H34" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
+    <hyperlink ref="J34" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K34" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L34" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="M34" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="N34" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="O34" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="M35" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H47" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
+    <hyperlink ref="H48" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
+    <hyperlink ref="I47" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor"/>
+    <hyperlink ref="I48" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor"/>
+    <hyperlink ref="J47" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
+    <hyperlink ref="J48" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
+    <hyperlink ref="G47" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G48" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G49" location="'ic_SubscribeNews_DupliEmailID++'!A1" display="ic_SubscribeNews_DupliEmailID"/>
+    <hyperlink ref="I40" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="G40" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H41" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="J40" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K40" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L40" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="M40" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="N40" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="Q40" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G41:G42" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="I41:I42" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="H40:H42" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="J40:J42" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K40:K42" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L40:L42" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="M40:M42" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="N40:N42" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="Q40:Q42" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="H54" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="M47" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N47" location="'CreditApp_NavigateFilter++'!A1" display="CreditApp_NavigateFilter"/>
+    <hyperlink ref="O47" location="'CreditStatusVerification++'!A1" display="CreditStatusVerification"/>
+    <hyperlink ref="N32" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="J2" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="J16:J21" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="P32" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="P40:P42" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="L48" location="'EnterContact++'!A1" display="EnterContact"/>
+    <hyperlink ref="L47" location="'EnterContact++'!A1" display="EnterContact"/>
+    <hyperlink ref="K48" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
+    <hyperlink ref="K47" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
+    <hyperlink ref="G39" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G38" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G53:G54" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="H53" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="I54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="I53" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="J54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="G35" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
+    <hyperlink ref="H35" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="I35" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="J35" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="K35" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="L35" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="G36" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H36" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard"/>
+    <hyperlink ref="I36" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="J36" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K37" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="I37" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard"/>
+    <hyperlink ref="K36" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L37" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="H38" location="'giftCardReport++'!A1" display="giftCardReport"/>
+    <hyperlink ref="H39" location="'giftCardReport++'!A1" display="giftCardReport"/>
+    <hyperlink ref="G50" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy"/>
+    <hyperlink ref="G50:G52" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy"/>
+    <hyperlink ref="J3:J6" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5614,29 +5588,29 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F05AC00-E67C-416B-8EF2-B4F01DABC1A7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" style="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" style="40" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.26953125" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" style="40" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.453125" style="40" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.1796875" style="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="40" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" style="40" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.7265625" style="40" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="40"/>
+    <col min="13" max="13" width="17.7109375" style="40" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -5770,10 +5744,10 @@
     <cfRule type="duplicateValues" dxfId="30" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{9D38FBF3-3229-4DF9-A60C-7C4E847C37CE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Ms,Mr,Dr,Miss,Mrs,Prof,Rev,Adv,Honorable"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{917AC3F9-CF96-4F34-9B10-8165C271324F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
       <formula1>"Female,Male"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5782,25 +5756,25 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E89C95-8E57-40B6-AD79-9CF25EBD0204}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" style="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.26953125" style="40" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.1796875" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.81640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="40"/>
+    <col min="4" max="4" width="22.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" style="40" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5898,13 +5872,13 @@
     <cfRule type="duplicateValues" dxfId="28" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{F7E2A111-1E7E-4D5A-998A-131FD5F11571}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{59795136-B460-4812-BE13-A22FF735B5DD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
       <formula1>"ABSA,AFRICAN BANK,BIDVEST.CAPITEC,FNB,INVESTEC,NEDBANK,STANDARD BANK SA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{22471F3C-77F9-4016-9487-42BDC823AD67}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576">
       <formula1>"English,Afrikaans,Sesotho,Xhosa,Zulu"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5913,28 +5887,28 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3BBBC42-3B7B-459B-B9B5-F7E2D92D455F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" style="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="40" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" style="40" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.26953125" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="40" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="40" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" style="40" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.453125" style="40" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.54296875" style="40" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="40"/>
+    <col min="10" max="10" width="11.7109375" style="40" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="40" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -6050,7 +6024,7 @@
     <cfRule type="duplicateValues" dxfId="26" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{FBD02F12-7E64-474D-BBAF-C36901F4E874}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
       <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6058,7 +6032,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AB4EACC7-1F75-483E-B43D-00C91A042EA6}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Preferred Store'!$A$2:$A$71</xm:f>
           </x14:formula1>
@@ -6071,24 +6045,24 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE12F75-2466-43A8-9ACA-6FC0C5879902}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.54296875" style="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="40" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" style="40" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="40"/>
+    <col min="8" max="8" width="18.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -6177,7 +6151,7 @@
     <cfRule type="duplicateValues" dxfId="24" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{142403CE-862D-4BAA-9115-F26CC2628162}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Domestic Worker,Company Employed,Government Employed,Full-time Housewife,Self Employed - Company Owner,Self Employed - Informal Trader,Student,Unemployed,Pensioner/Retired,Contract Worker,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6187,38 +6161,38 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA138F04-FB51-4E31-A7CF-C182781998FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="40" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.81640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.81640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.81640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.1796875" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.453125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.42578125" style="40" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" style="40" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.1796875" style="40" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="40" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" style="40" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1796875" style="40"/>
-    <col min="15" max="15" width="23.81640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.54296875" style="40" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.81640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7265625" style="40" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.1796875" style="40" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.54296875" style="40" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.54296875" style="40" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.7265625" style="40" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.1796875" style="40"/>
+    <col min="14" max="14" width="9.140625" style="40"/>
+    <col min="15" max="15" width="23.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" style="40" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" style="40" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" style="40" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" style="40" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.5703125" style="40" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" style="40" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -6433,25 +6407,25 @@
     <cfRule type="duplicateValues" dxfId="22" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3" xr:uid="{BB169D04-5A5B-481D-BD2C-71560D21535F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3" xr:uid="{4A3826AF-7254-495C-BEBC-3F323EA2C87D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3">
       <formula1>"Ms,Mr,Dr,Miss,Mrs,Prof,Rev,Adv,Honorable"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3" xr:uid="{F982BA19-EEA6-45AC-8A6E-E813B802787D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3">
       <formula1>"African,Asian,Coloured,White,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3" xr:uid="{76A667A8-2B5B-43EC-816B-D731AA0010D7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3">
       <formula1>"Single,Married / Civil Partnership,Widowed,Divorced,Separated,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3" xr:uid="{FE30C889-C167-4151-96A0-2D206E891DD9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3">
       <formula1>"ANC with Accrual,ANC without Accrual,In Community,Customary Union,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U3" xr:uid="{43E6CA37-94A1-41E3-8591-A9C16AADB817}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U3">
       <formula1>"Female,Male"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576" xr:uid="{57467C3F-7191-4E96-B459-B86A1BFA06D5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576">
       <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6461,22 +6435,22 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1796875" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.81640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" style="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="40"/>
+    <col min="4" max="4" width="20.140625" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="40" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -6532,17 +6506,17 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="39" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="39" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="39"/>
@@ -6589,25 +6563,25 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.1796875" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="33" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" style="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1796875" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" style="33" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" style="33" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="33"/>
+    <col min="10" max="16384" width="9.140625" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -6680,10 +6654,10 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H2" sqref="H2"/>
       <selection pane="topRight" activeCell="H2" sqref="H2"/>
@@ -6691,42 +6665,42 @@
       <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" style="11" customWidth="1"/>
-    <col min="14" max="14" width="20.26953125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="31.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="11" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" style="11" customWidth="1"/>
+    <col min="15" max="15" width="31.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="30" style="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="30.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="20" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="27.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.1796875" style="11" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="11.54296875" style="11" customWidth="1"/>
-    <col min="31" max="16384" width="8.7265625" style="11"/>
+    <col min="27" max="27" width="23.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="27.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.140625" style="11" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="11.5703125" style="11" customWidth="1"/>
+    <col min="31" max="16384" width="8.7109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" ht="30">
       <c r="A1" s="17" t="s">
         <v>34</v>
       </c>
@@ -7162,7 +7136,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:28" s="33" customFormat="1" ht="16" customHeight="1">
+    <row r="9" spans="1:28" s="33" customFormat="1" ht="15.95" customHeight="1">
       <c r="A9" s="18">
         <v>2</v>
       </c>
@@ -7212,7 +7186,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:28" s="33" customFormat="1" ht="16" customHeight="1">
+    <row r="10" spans="1:28" s="33" customFormat="1" ht="15.95" customHeight="1">
       <c r="A10" s="18">
         <v>5</v>
       </c>
@@ -7262,7 +7236,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:28" s="33" customFormat="1" ht="16" customHeight="1">
+    <row r="11" spans="1:28" s="33" customFormat="1" ht="15.95" customHeight="1">
       <c r="A11" s="18">
         <v>6</v>
       </c>
@@ -7312,7 +7286,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="33" customFormat="1" ht="16" customHeight="1">
+    <row r="12" spans="1:28" s="33" customFormat="1" ht="15.95" customHeight="1">
       <c r="A12" s="18">
         <v>9</v>
       </c>
@@ -7362,7 +7336,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:28" s="33" customFormat="1" ht="16" customHeight="1">
+    <row r="13" spans="1:28" s="33" customFormat="1" ht="15.95" customHeight="1">
       <c r="A13" s="18">
         <v>3</v>
       </c>
@@ -7414,69 +7388,69 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q13 Y3:Y13" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q13 Y3:Y13">
       <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F13 I2:I13 K2:K13 M2:O13 G2:G13 E2:E13 U2:W13" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F13 I2:I13 K2:K13 M2:O13 G2:G13 E2:E13 U2:W13">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="D6:D7" r:id="rId2" display="original2Ic@automationjdg.co.za" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="D7" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="D2:D4" r:id="rId4" display="original2Ic@automationjdg.co.za" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="D8" r:id="rId5" xr:uid="{D9F460A3-6579-42AC-B134-23192575BB73}"/>
-    <hyperlink ref="D9" r:id="rId6" xr:uid="{ACEAAFEE-EB40-4EFB-A421-EEE4EF67DC8E}"/>
-    <hyperlink ref="D10" r:id="rId7" xr:uid="{A466288E-BE8F-42DF-8E63-90DC83FBD555}"/>
-    <hyperlink ref="D11" r:id="rId8" xr:uid="{1ED175BB-E356-4421-9580-06B490802E99}"/>
-    <hyperlink ref="D12" r:id="rId9" xr:uid="{68C96D03-3D77-41F0-83D7-042AEE01849A}"/>
-    <hyperlink ref="D13" r:id="rId10" xr:uid="{D563E716-EB3C-44C8-975E-C7E1BEAFAF17}"/>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="D6:D7" r:id="rId2" display="original2Ic@automationjdg.co.za"/>
+    <hyperlink ref="D7" r:id="rId3"/>
+    <hyperlink ref="D2:D4" r:id="rId4" display="original2Ic@automationjdg.co.za"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+    <hyperlink ref="D9" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+    <hyperlink ref="D11" r:id="rId8"/>
+    <hyperlink ref="D12" r:id="rId9"/>
+    <hyperlink ref="D13" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC13"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.54296875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7265625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.81640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.26953125" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.54296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.54296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18" style="12" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="21" style="12" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="25" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.81640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="30" style="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.7265625" style="12" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="30.26953125" style="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.1796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="27.1796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="8.7265625" style="12"/>
+    <col min="28" max="28" width="23.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="27.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="8.7109375" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -8084,7 +8058,7 @@
       <c r="AB11" s="16"/>
       <c r="AC11" s="16"/>
     </row>
-    <row r="12" spans="1:29" s="35" customFormat="1" ht="16" customHeight="1">
+    <row r="12" spans="1:29" s="35" customFormat="1" ht="15.95" customHeight="1">
       <c r="A12" s="18">
         <v>9</v>
       </c>
@@ -8188,7 +8162,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8197,19 +8171,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C3EA7E-59AC-4978-BC40-C9AB85C8600E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.81640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.1796875" style="40"/>
+    <col min="4" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -8257,7 +8231,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8268,14 +8242,14 @@
       <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -8711,7 +8685,7 @@
     <cfRule type="duplicateValues" dxfId="16" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Guest Customer Creation, Customer Creation, Customer Update,Customer Creation Magento Admin, Customer Update Magento Admin"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8720,22 +8694,22 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -8889,26 +8863,26 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="42" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.26953125" style="42" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="42" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.54296875" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="42" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" style="42" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" style="42" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="42" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="42" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="42"/>
+    <col min="11" max="16384" width="9.140625" style="42"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="70" customFormat="1">
@@ -9338,19 +9312,19 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -9568,7 +9542,7 @@
     <cfRule type="duplicateValues" dxfId="14" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"payUcreditcard,Cash_Deposits"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9577,33 +9551,33 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.81640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="29">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="30">
       <c r="A1" s="41" t="s">
         <v>34</v>
       </c>
@@ -10477,14 +10451,14 @@
     <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
-    <hyperlink ref="O3" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
-    <hyperlink ref="O4" r:id="rId3" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
-    <hyperlink ref="O5" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
-    <hyperlink ref="O8" r:id="rId5" xr:uid="{00000000-0004-0000-0A00-000004000000}"/>
-    <hyperlink ref="O6" r:id="rId6" xr:uid="{00000000-0004-0000-0A00-000005000000}"/>
-    <hyperlink ref="O7" r:id="rId7" xr:uid="{00000000-0004-0000-0A00-000006000000}"/>
-    <hyperlink ref="O9" r:id="rId8" xr:uid="{00000000-0004-0000-0A00-000007000000}"/>
+    <hyperlink ref="O2" r:id="rId1"/>
+    <hyperlink ref="O3" r:id="rId2"/>
+    <hyperlink ref="O4" r:id="rId3"/>
+    <hyperlink ref="O5" r:id="rId4"/>
+    <hyperlink ref="O8" r:id="rId5"/>
+    <hyperlink ref="O6" r:id="rId6"/>
+    <hyperlink ref="O7" r:id="rId7"/>
+    <hyperlink ref="O9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
@@ -10492,27 +10466,27 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.54296875" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="6"/>
+    <col min="4" max="4" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -10657,31 +10631,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000004000000}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-0B00-000005000000}"/>
-    <hyperlink ref="J3" r:id="rId3" xr:uid="{00000000-0004-0000-0B00-000006000000}"/>
-    <hyperlink ref="H3" r:id="rId4" xr:uid="{00000000-0004-0000-0B00-000007000000}"/>
-    <hyperlink ref="J4" r:id="rId5" xr:uid="{00000000-0004-0000-0B00-000008000000}"/>
-    <hyperlink ref="H4" r:id="rId6" xr:uid="{00000000-0004-0000-0B00-000009000000}"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
+    <hyperlink ref="J3" r:id="rId3"/>
+    <hyperlink ref="H3" r:id="rId4"/>
+    <hyperlink ref="J4" r:id="rId5"/>
+    <hyperlink ref="H4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -10698,7 +10672,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29">
+    <row r="2" spans="1:4" ht="30">
       <c r="A2" s="18">
         <v>26</v>
       </c>
@@ -10712,7 +10686,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="43.5">
+    <row r="3" spans="1:4" s="1" customFormat="1" ht="45">
       <c r="A3" s="18">
         <v>27</v>
       </c>
@@ -10726,7 +10700,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="43.5">
+    <row r="4" spans="1:4" ht="45">
       <c r="A4" s="18">
         <v>28</v>
       </c>
@@ -10740,7 +10714,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="29">
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" s="18">
         <v>29</v>
       </c>
@@ -10754,7 +10728,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="29">
+    <row r="6" spans="1:4" ht="30">
       <c r="A6" s="18">
         <v>30</v>
       </c>
@@ -10768,7 +10742,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="29">
+    <row r="7" spans="1:4" ht="30">
       <c r="A7" s="18">
         <v>31</v>
       </c>
@@ -10878,21 +10852,21 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -11140,21 +11114,21 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="42" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="42" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="42"/>
+    <col min="5" max="5" width="13.5703125" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="42"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -11234,7 +11208,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="18">
         <v>30</v>
       </c>
@@ -11369,7 +11343,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11380,14 +11354,14 @@
       <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="1"/>
+    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12025,20 +11999,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{742AE036-2668-4F56-9ABD-EF14E9F06100}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.81640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.26953125" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="40"/>
+    <col min="4" max="4" width="19.28515625" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -12091,7 +12065,7 @@
     <cfRule type="duplicateValues" dxfId="43" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{5A9BC578-1E6D-4437-94ED-17B8FB19B57A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
       <formula1>"All,Specific"</formula1>
     </dataValidation>
   </dataValidations>
@@ -12100,7 +12074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12110,13 +12084,13 @@
       <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="11"/>
+    <col min="4" max="4" width="7.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -12133,7 +12107,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29">
+    <row r="2" spans="1:4" ht="30">
       <c r="A2" s="18">
         <v>26</v>
       </c>
@@ -12145,7 +12119,7 @@
       </c>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:4" ht="43.5">
+    <row r="3" spans="1:4" ht="45">
       <c r="A3" s="18">
         <v>27</v>
       </c>
@@ -12157,7 +12131,7 @@
       </c>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="1:4" ht="43.5">
+    <row r="4" spans="1:4" ht="45">
       <c r="A4" s="18">
         <v>28</v>
       </c>
@@ -12169,7 +12143,7 @@
       </c>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:4" ht="29">
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" s="18">
         <v>29</v>
       </c>
@@ -12181,7 +12155,7 @@
       </c>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="1:4" ht="29">
+    <row r="6" spans="1:4" ht="30">
       <c r="A6" s="18">
         <v>30</v>
       </c>
@@ -12193,7 +12167,7 @@
       </c>
       <c r="D6" s="18"/>
     </row>
-    <row r="7" spans="1:4" ht="29">
+    <row r="7" spans="1:4" ht="30">
       <c r="A7" s="18">
         <v>31</v>
       </c>
@@ -12265,7 +12239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -12275,23 +12249,23 @@
       <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="73" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="73" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="73" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="73" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" style="73" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.453125" style="73" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.54296875" style="73" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" style="73" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="73" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.7265625" style="73" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.26953125" style="73" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="73" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" style="73" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="73" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="73" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="73" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" style="73" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" style="73" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2" style="73" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="73"/>
+    <col min="12" max="16384" width="9.140625" style="73"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" ht="30">
       <c r="A1" s="72" t="s">
         <v>34</v>
       </c>
@@ -12387,7 +12361,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="43.5">
+    <row r="4" spans="1:10" ht="45">
       <c r="A4" s="74">
         <v>28</v>
       </c>
@@ -12719,13 +12693,13 @@
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G13" xr:uid="{1931666E-9688-4D00-8471-B4031677CC66}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G13">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F13" xr:uid="{96A31591-7DD4-4C3E-BCD8-B3DDCB5C36EB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F13">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J13" xr:uid="{AA5BEE0A-3E01-4DBF-BD84-D7ADD2A6E726}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J13">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
     </dataValidation>
   </dataValidations>
@@ -12735,13 +12709,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D940762B-C385-42F6-A68B-0567064BCC3E}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Products_Category!$A$2:$A$18</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D13</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{485622A6-79DB-4819-8FA7-E869A5D8141C}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Products_Category!$A$2:$A$7</xm:f>
           </x14:formula1>
@@ -12754,16 +12728,16 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79FC64ED-B07B-4692-B6D1-76EE75EB9E3E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.26953125" style="42" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" style="42" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -12862,21 +12836,21 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" style="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="35"/>
+    <col min="4" max="4" width="18.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12937,21 +12911,21 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -13021,21 +12995,21 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="1"/>
+    <col min="5" max="5" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -13288,16 +13262,16 @@
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
-    <hyperlink ref="E6" r:id="rId2" xr:uid="{00000000-0004-0000-1400-000001000000}"/>
-    <hyperlink ref="E7" r:id="rId3" xr:uid="{00000000-0004-0000-1400-000002000000}"/>
-    <hyperlink ref="E8" r:id="rId4" xr:uid="{00000000-0004-0000-1400-000003000000}"/>
-    <hyperlink ref="E9" r:id="rId5" xr:uid="{00000000-0004-0000-1400-000004000000}"/>
-    <hyperlink ref="E10" r:id="rId6" xr:uid="{00000000-0004-0000-1400-000005000000}"/>
-    <hyperlink ref="E11" r:id="rId7" xr:uid="{00000000-0004-0000-1400-000006000000}"/>
-    <hyperlink ref="E12" r:id="rId8" xr:uid="{6F0053FF-EDC0-42B0-BAC2-03BC906EB334}"/>
-    <hyperlink ref="E13" r:id="rId9" xr:uid="{4285B4A6-FF82-44A1-8801-840C01253369}"/>
-    <hyperlink ref="E14" r:id="rId10" xr:uid="{749BA145-53D9-4017-A849-9C0A68E385B8}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E6" r:id="rId2"/>
+    <hyperlink ref="E7" r:id="rId3"/>
+    <hyperlink ref="E8" r:id="rId4"/>
+    <hyperlink ref="E9" r:id="rId5"/>
+    <hyperlink ref="E10" r:id="rId6"/>
+    <hyperlink ref="E11" r:id="rId7"/>
+    <hyperlink ref="E12" r:id="rId8"/>
+    <hyperlink ref="E13" r:id="rId9"/>
+    <hyperlink ref="E14" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
@@ -13305,21 +13279,21 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -13409,7 +13383,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -13417,26 +13391,26 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -13515,19 +13489,19 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1">
@@ -13561,31 +13535,31 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="1"/>
+    <col min="12" max="12" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29">
+    <row r="1" spans="1:12" ht="30">
       <c r="A1" s="17" t="s">
         <v>34</v>
       </c>
@@ -13623,7 +13597,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" ht="30">
       <c r="A2" s="18">
         <v>6</v>
       </c>
@@ -13657,7 +13631,7 @@
       </c>
       <c r="L2" s="18"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" ht="30">
       <c r="A3" s="18">
         <v>7</v>
       </c>
@@ -13691,7 +13665,7 @@
       </c>
       <c r="L3" s="18"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" s="18">
         <v>8</v>
       </c>
@@ -13725,7 +13699,7 @@
       </c>
       <c r="L4" s="18"/>
     </row>
-    <row r="5" spans="1:12" s="33" customFormat="1">
+    <row r="5" spans="1:12" s="33" customFormat="1" ht="30">
       <c r="A5" s="18">
         <v>1</v>
       </c>
@@ -13759,7 +13733,7 @@
       </c>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" spans="1:12" s="33" customFormat="1">
+    <row r="6" spans="1:12" s="33" customFormat="1" ht="30">
       <c r="A6" s="18">
         <v>2</v>
       </c>
@@ -13793,7 +13767,7 @@
       </c>
       <c r="L6" s="18"/>
     </row>
-    <row r="7" spans="1:12" s="33" customFormat="1">
+    <row r="7" spans="1:12" s="33" customFormat="1" ht="30">
       <c r="A7" s="18">
         <v>1</v>
       </c>
@@ -13863,7 +13837,7 @@
       </c>
       <c r="L8" s="18"/>
     </row>
-    <row r="9" spans="1:12" s="33" customFormat="1" ht="17" customHeight="1">
+    <row r="9" spans="1:12" s="33" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="18">
         <v>9</v>
       </c>
@@ -13980,23 +13954,23 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J10" xr:uid="{00000000-0002-0000-1800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J10">
       <formula1>"Main Website,Incredible Connection"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G10 F11:F1048576" xr:uid="{00000000-0002-0000-1800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G10 F11:F1048576">
       <formula1>"SAID,Passport"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-1800-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-1800-000002000000}"/>
-    <hyperlink ref="F5" r:id="rId4" display="TestAutomation2@gmail.com" xr:uid="{C0AFDD72-4B3D-420D-8B0F-7AD98D29D52C}"/>
-    <hyperlink ref="F6" r:id="rId5" display="TestAutomation2@gmail.com" xr:uid="{92B3A593-D32F-4A80-8673-BC70657B5E7F}"/>
-    <hyperlink ref="F7" r:id="rId6" display="TestAutomation2@gmail.com" xr:uid="{5AD50CC3-819C-4E82-AD73-98F922ABD99D}"/>
-    <hyperlink ref="F8" r:id="rId7" display="TestAutomation2@gmail.com" xr:uid="{385CB16C-F360-40A0-BB9E-61E91B37FC42}"/>
-    <hyperlink ref="F9" r:id="rId8" display="TestAutomation2@gmail.com" xr:uid="{DA39F455-083E-430F-AD35-9AFC0110AC38}"/>
-    <hyperlink ref="F10" r:id="rId9" display="TestAutomation2@gmail.com" xr:uid="{B7395BA8-34EB-4EE0-86D9-36B1B9005493}"/>
+    <hyperlink ref="F2" r:id="rId1" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F3" r:id="rId2" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F4" r:id="rId3" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F5" r:id="rId4" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F6" r:id="rId5" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F7" r:id="rId6" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F8" r:id="rId7" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F9" r:id="rId8" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F10" r:id="rId9" display="TestAutomation2@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
@@ -14005,23 +13979,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3713ADE9-FAFA-4360-B995-9E201E975715}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.81640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="40" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="40" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="40" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="40"/>
+    <col min="8" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -14101,34 +14075,34 @@
     <cfRule type="duplicateValues" dxfId="41" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{DECB0F6A-3521-4D27-A6E3-16253250FAD6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
       <formula1>"ExistingUser,logedOn_user"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{B6DECD2A-3DC5-4E0C-B54A-F5A3F07D00AD}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{0F9905DC-3EC1-4B39-91DE-85D98BF9759D}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
@@ -14218,19 +14192,19 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1">
@@ -14422,21 +14396,21 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -14526,21 +14500,21 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -14630,16 +14604,16 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8325266A-E78C-4F11-89FB-0C8A2E994631}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -15003,21 +14977,21 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -15107,21 +15081,21 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="L14" workbookViewId="0">
       <selection activeCell="Y27" sqref="Y27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -15211,20 +15185,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920941E8-63A8-46DF-9CEB-D9EA33709737}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="63" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="63" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="63" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="63" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" style="63" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="63"/>
+    <col min="5" max="16384" width="9.140625" style="63"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -15597,7 +15571,7 @@
     <cfRule type="duplicateValues" dxfId="35" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{D81566CD-2D7F-4343-99FF-D070BCA691BE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Update Account,Update Account Magento Admin,Create Account,Create Account Magento Admin,Guest Customer Creation,Registered customer from sales order"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15606,21 +15580,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49ACECBA-0977-4B07-97CF-646D9D65E402}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="40"/>
+    <col min="4" max="4" width="11.5703125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -15700,38 +15674,38 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD40FD6A-3206-4F33-9099-D76F7461AC19}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T4" sqref="T4"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" style="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.7265625" style="33" customWidth="1"/>
-    <col min="3" max="4" width="10.81640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7265625" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.81640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" style="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.81640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" style="33" customWidth="1"/>
+    <col min="3" max="4" width="10.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" style="33" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" style="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7265625" style="33" customWidth="1"/>
-    <col min="12" max="12" width="23.1796875" style="33" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7265625" style="33" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.1796875" style="33" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.453125" style="33" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.81640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.81640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.54296875" style="33" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.26953125" style="33" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.1796875" style="33" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.1796875" style="33"/>
+    <col min="10" max="10" width="11.7109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="33" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -15796,7 +15770,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="29">
+    <row r="2" spans="1:20" ht="30">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -15858,7 +15832,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="29">
+    <row r="3" spans="1:20" ht="30">
       <c r="A3" s="18">
         <v>2</v>
       </c>
@@ -15920,7 +15894,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="29">
+    <row r="4" spans="1:20" ht="30">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -15982,7 +15956,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="29">
+    <row r="5" spans="1:20" ht="30">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -16042,7 +16016,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="29">
+    <row r="6" spans="1:20" ht="30">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -16104,7 +16078,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="43.5">
+    <row r="7" spans="1:20" ht="45">
       <c r="A7" s="18">
         <v>21</v>
       </c>
@@ -16164,7 +16138,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="29">
+    <row r="8" spans="1:20" ht="30">
       <c r="A8" s="18">
         <v>22</v>
       </c>
@@ -16224,7 +16198,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="43.5">
+    <row r="9" spans="1:20" ht="45">
       <c r="A9" s="18">
         <v>23</v>
       </c>
@@ -16284,7 +16258,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="43.5">
+    <row r="10" spans="1:20" ht="45">
       <c r="A10" s="18">
         <v>24</v>
       </c>
@@ -16344,7 +16318,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="29">
+    <row r="11" spans="1:20" ht="30">
       <c r="A11" s="18">
         <v>25</v>
       </c>
@@ -16404,7 +16378,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="29">
+    <row r="12" spans="1:20" ht="30">
       <c r="A12" s="18">
         <v>6</v>
       </c>
@@ -16464,7 +16438,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="29">
+    <row r="13" spans="1:20" ht="30">
       <c r="A13" s="18">
         <v>9</v>
       </c>
@@ -16526,16 +16500,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M13" xr:uid="{FF70BC0E-3989-4E4A-9EDB-1D6DA4A25EBB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M13">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N13" xr:uid="{D81261F8-C548-4AA4-9D26-48EC0E008ACF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N13">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I13 P2:T13" xr:uid="{9A1E9D13-8395-4C31-BF32-7E3AFBE71119}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I13 P2:T13">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L13" xr:uid="{26B96BFD-6003-4E83-A937-3CEE292F260C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L13">
       <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
     </dataValidation>
   </dataValidations>
@@ -16545,21 +16519,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0765784-E02D-42F9-B37F-9F1A7F613903}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.453125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.42578125" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="40"/>
+    <col min="4" max="4" width="15.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -16608,20 +16582,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7D9075-5F21-450D-8059-BA8C0176E98B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="40"/>
-    <col min="2" max="2" width="14.08984375" style="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.453125" style="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="40"/>
+    <col min="1" max="1" width="8.7109375" style="40"/>
+    <col min="2" max="2" width="14.140625" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -16708,15 +16682,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16865,6 +16830,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
@@ -16874,23 +16848,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16907,4 +16864,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TCID 1 to 12 fixes included
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupUpdated.xlsx
+++ b/src/test/resources/data/jdgroupUpdated.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6AAFF6-0504-485A-8DBE-F800BD1A9FE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB6CBE3-11F9-43F8-B9B1-8165588A361F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3510" yWindow="-10910" windowWidth="19420" windowHeight="10420" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2545" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2638" uniqueCount="649">
   <si>
     <t>testSuitID</t>
   </si>
@@ -2034,6 +2034,54 @@
   </si>
   <si>
     <t>BackendLastName</t>
+  </si>
+  <si>
+    <t>45 Pritchard Street</t>
+  </si>
+  <si>
+    <t>0670441106</t>
+  </si>
+  <si>
+    <t>abcd1241</t>
+  </si>
+  <si>
+    <t>12 James Street</t>
+  </si>
+  <si>
+    <t>GuestCust</t>
+  </si>
+  <si>
+    <t>LastNameGuest</t>
+  </si>
+  <si>
+    <t>Germiston</t>
+  </si>
+  <si>
+    <t>Durban</t>
+  </si>
+  <si>
+    <t>4352</t>
+  </si>
+  <si>
+    <t>578375</t>
+  </si>
+  <si>
+    <t>guestCust@jdg.co.za</t>
+  </si>
+  <si>
+    <t>9306201438084</t>
+  </si>
+  <si>
+    <t>Action12</t>
+  </si>
+  <si>
+    <t>abcd1242</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>0857389235</t>
   </si>
 </sst>
 </file>
@@ -3276,11 +3324,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R55"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="M23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomRight" activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -3289,7 +3337,7 @@
     <col min="2" max="2" width="93.54296875" style="58" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.26953125" style="58" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="90.7265625" style="58" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" style="58" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" style="58" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.81640625" style="58" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="33.7265625" style="58" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.81640625" style="58" bestFit="1" customWidth="1"/>
@@ -3302,7 +3350,7 @@
     <col min="18" max="16384" width="9.1796875" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="41" t="s">
         <v>15</v>
       </c>
@@ -3354,8 +3402,11 @@
       <c r="Q1" s="41" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" ht="29">
+      <c r="R1" s="58" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="29">
       <c r="A2" s="50">
         <v>1</v>
       </c>
@@ -3396,7 +3447,7 @@
       <c r="P2" s="50"/>
       <c r="Q2" s="50"/>
     </row>
-    <row r="3" spans="1:17" ht="29">
+    <row r="3" spans="1:18" ht="29">
       <c r="A3" s="50">
         <v>2</v>
       </c>
@@ -3437,7 +3488,7 @@
       <c r="P3" s="50"/>
       <c r="Q3" s="50"/>
     </row>
-    <row r="4" spans="1:17" ht="29">
+    <row r="4" spans="1:18" ht="29">
       <c r="A4" s="50">
         <v>3</v>
       </c>
@@ -3478,7 +3529,7 @@
       <c r="P4" s="50"/>
       <c r="Q4" s="50"/>
     </row>
-    <row r="5" spans="1:17" ht="29">
+    <row r="5" spans="1:18" ht="29">
       <c r="A5" s="50">
         <v>4</v>
       </c>
@@ -3519,7 +3570,7 @@
       <c r="P5" s="50"/>
       <c r="Q5" s="50"/>
     </row>
-    <row r="6" spans="1:17" ht="29">
+    <row r="6" spans="1:18" ht="29">
       <c r="A6" s="50">
         <v>5</v>
       </c>
@@ -3560,7 +3611,7 @@
       <c r="P6" s="50"/>
       <c r="Q6" s="50"/>
     </row>
-    <row r="7" spans="1:17" ht="29">
+    <row r="7" spans="1:18" ht="29">
       <c r="A7" s="50">
         <v>6</v>
       </c>
@@ -3599,7 +3650,7 @@
       <c r="P7" s="50"/>
       <c r="Q7" s="50"/>
     </row>
-    <row r="8" spans="1:17" ht="29">
+    <row r="8" spans="1:18" ht="29">
       <c r="A8" s="50">
         <v>7</v>
       </c>
@@ -3638,7 +3689,7 @@
       <c r="P8" s="50"/>
       <c r="Q8" s="50"/>
     </row>
-    <row r="9" spans="1:17" ht="29">
+    <row r="9" spans="1:18" ht="29">
       <c r="A9" s="50">
         <v>8</v>
       </c>
@@ -3677,7 +3728,7 @@
       <c r="P9" s="50"/>
       <c r="Q9" s="50"/>
     </row>
-    <row r="10" spans="1:17" ht="29">
+    <row r="10" spans="1:18" ht="29">
       <c r="A10" s="50">
         <v>9</v>
       </c>
@@ -3691,7 +3742,7 @@
         <v>220</v>
       </c>
       <c r="E10" s="50" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F10" s="51" t="s">
         <v>199</v>
@@ -3716,7 +3767,7 @@
       <c r="P10" s="50"/>
       <c r="Q10" s="50"/>
     </row>
-    <row r="11" spans="1:17" ht="29">
+    <row r="11" spans="1:18" ht="29">
       <c r="A11" s="50">
         <v>10</v>
       </c>
@@ -3755,7 +3806,7 @@
       <c r="P11" s="50"/>
       <c r="Q11" s="50"/>
     </row>
-    <row r="12" spans="1:17" ht="29">
+    <row r="12" spans="1:18" ht="29">
       <c r="A12" s="50">
         <v>11</v>
       </c>
@@ -3794,7 +3845,7 @@
       <c r="P12" s="50"/>
       <c r="Q12" s="50"/>
     </row>
-    <row r="13" spans="1:17" ht="29">
+    <row r="13" spans="1:18" ht="29">
       <c r="A13" s="50">
         <v>12</v>
       </c>
@@ -3833,7 +3884,7 @@
       <c r="P13" s="50"/>
       <c r="Q13" s="50"/>
     </row>
-    <row r="14" spans="1:17" ht="29">
+    <row r="14" spans="1:18" ht="29">
       <c r="A14" s="50">
         <v>13</v>
       </c>
@@ -3872,7 +3923,7 @@
       <c r="P14" s="50"/>
       <c r="Q14" s="50"/>
     </row>
-    <row r="15" spans="1:17" ht="29">
+    <row r="15" spans="1:18" ht="29">
       <c r="A15" s="50">
         <v>14</v>
       </c>
@@ -3911,7 +3962,7 @@
       <c r="P15" s="50"/>
       <c r="Q15" s="50"/>
     </row>
-    <row r="16" spans="1:17" ht="29">
+    <row r="16" spans="1:18" ht="29">
       <c r="A16" s="50">
         <v>15</v>
       </c>
@@ -3952,7 +4003,7 @@
       <c r="P16" s="50"/>
       <c r="Q16" s="50"/>
     </row>
-    <row r="17" spans="1:18" ht="29">
+    <row r="17" spans="1:17" ht="29">
       <c r="A17" s="50">
         <v>16</v>
       </c>
@@ -3993,7 +4044,7 @@
       <c r="P17" s="50"/>
       <c r="Q17" s="50"/>
     </row>
-    <row r="18" spans="1:18" ht="29">
+    <row r="18" spans="1:17" ht="29">
       <c r="A18" s="50">
         <v>17</v>
       </c>
@@ -4034,7 +4085,7 @@
       <c r="P18" s="50"/>
       <c r="Q18" s="50"/>
     </row>
-    <row r="19" spans="1:18" ht="29">
+    <row r="19" spans="1:17" ht="29">
       <c r="A19" s="50">
         <v>18</v>
       </c>
@@ -4075,7 +4126,7 @@
       <c r="P19" s="50"/>
       <c r="Q19" s="50"/>
     </row>
-    <row r="20" spans="1:18" ht="29">
+    <row r="20" spans="1:17" ht="29">
       <c r="A20" s="50">
         <v>19</v>
       </c>
@@ -4116,7 +4167,7 @@
       <c r="P20" s="50"/>
       <c r="Q20" s="50"/>
     </row>
-    <row r="21" spans="1:18" ht="29">
+    <row r="21" spans="1:17" ht="29">
       <c r="A21" s="50">
         <v>20</v>
       </c>
@@ -4157,7 +4208,7 @@
       <c r="P21" s="50"/>
       <c r="Q21" s="50"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:17">
       <c r="A22" s="50">
         <v>21</v>
       </c>
@@ -4187,7 +4238,7 @@
       <c r="O22" s="50"/>
       <c r="P22" s="50"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:17">
       <c r="A23" s="50">
         <v>22</v>
       </c>
@@ -4217,7 +4268,7 @@
       <c r="O23" s="50"/>
       <c r="P23" s="50"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:17">
       <c r="A24" s="50">
         <v>23</v>
       </c>
@@ -4247,7 +4298,7 @@
       <c r="O24" s="50"/>
       <c r="P24" s="50"/>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:17">
       <c r="A25" s="50">
         <v>24</v>
       </c>
@@ -4277,7 +4328,7 @@
       <c r="O25" s="50"/>
       <c r="P25" s="50"/>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:17">
       <c r="A26" s="50">
         <v>25</v>
       </c>
@@ -4307,7 +4358,7 @@
       <c r="O26" s="50"/>
       <c r="P26" s="50"/>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:17">
       <c r="A27" s="50">
         <v>26</v>
       </c>
@@ -4353,7 +4404,7 @@
       </c>
       <c r="Q27" s="50"/>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:17">
       <c r="A28" s="50">
         <v>27</v>
       </c>
@@ -4399,7 +4450,7 @@
       </c>
       <c r="P28" s="50"/>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:17">
       <c r="A29" s="50">
         <v>28</v>
       </c>
@@ -4445,7 +4496,7 @@
       </c>
       <c r="P29" s="50"/>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:17">
       <c r="A30" s="50">
         <v>29</v>
       </c>
@@ -4491,7 +4542,7 @@
       </c>
       <c r="P30" s="50"/>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:17">
       <c r="A31" s="50">
         <v>30</v>
       </c>
@@ -4535,7 +4586,7 @@
       <c r="O31" s="50"/>
       <c r="P31" s="50"/>
     </row>
-    <row r="32" spans="1:18" ht="29">
+    <row r="32" spans="1:17">
       <c r="A32" s="50">
         <v>31</v>
       </c>
@@ -4547,7 +4598,7 @@
       </c>
       <c r="D32" s="50"/>
       <c r="E32" s="50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" s="51"/>
       <c r="G32" s="52" t="s">
@@ -4574,16 +4625,13 @@
       <c r="N32" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="O32" s="61" t="s">
-        <v>304</v>
+      <c r="O32" s="53" t="s">
+        <v>302</v>
       </c>
       <c r="P32" s="53" t="s">
-        <v>302</v>
+        <v>198</v>
       </c>
       <c r="Q32" s="53" t="s">
-        <v>198</v>
-      </c>
-      <c r="R32" s="53" t="s">
         <v>214</v>
       </c>
     </row>
@@ -5520,8 +5568,8 @@
     <hyperlink ref="J32" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0700-00006E000000}"/>
     <hyperlink ref="M32" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0700-00006F000000}"/>
     <hyperlink ref="K32" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0700-000070000000}"/>
-    <hyperlink ref="Q32" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0700-000071000000}"/>
-    <hyperlink ref="R32" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0700-000072000000}"/>
+    <hyperlink ref="P32" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0700-000071000000}"/>
+    <hyperlink ref="Q32" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0700-000072000000}"/>
     <hyperlink ref="G34" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0700-000073000000}"/>
     <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0700-000074000000}"/>
     <hyperlink ref="H37" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0700-000075000000}"/>
@@ -5575,7 +5623,7 @@
     <hyperlink ref="N32" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0700-00006C000000}"/>
     <hyperlink ref="J2" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{41A192C1-C805-44EA-A5B1-D5BFEDEE0CA8}"/>
     <hyperlink ref="J16:J21" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{E117577A-CEDC-4A1C-88A3-6B50A0AB895E}"/>
-    <hyperlink ref="P32" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{AE5A2668-9089-474A-8EDC-8C5E743A4780}"/>
+    <hyperlink ref="O32" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{AE5A2668-9089-474A-8EDC-8C5E743A4780}"/>
     <hyperlink ref="P40:P42" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{DEC89986-4AC0-45D7-81DD-64BB1C3C9DA9}"/>
     <hyperlink ref="L48" location="'EnterContact++'!A1" display="EnterContact" xr:uid="{00000000-0004-0000-0700-00008F000000}"/>
     <hyperlink ref="L47" location="'EnterContact++'!A1" display="EnterContact" xr:uid="{00000000-0004-0000-0700-00008E000000}"/>
@@ -6681,14 +6729,14 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AC13"/>
+  <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H2" sqref="H2"/>
       <selection pane="topRight" activeCell="H2" sqref="H2"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -7023,7 +7071,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>255</v>
+        <v>617</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>92</v>
@@ -7034,7 +7082,7 @@
       </c>
       <c r="H6" s="18"/>
       <c r="I6" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J6" s="18"/>
       <c r="K6" s="18" t="s">
@@ -7412,12 +7460,62 @@
         <v>92</v>
       </c>
     </row>
+    <row r="14" spans="1:28" s="33" customFormat="1" ht="16" customHeight="1">
+      <c r="A14" s="18">
+        <v>31</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>616</v>
+      </c>
+      <c r="C14" s="18">
+        <v>1</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>617</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="N14" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18" t="s">
+        <v>615</v>
+      </c>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="V14" s="33" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q13 Y3:Y13" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q14 Y3:Y14" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F13 I2:I13 K2:K13 M2:O13 G2:G13 E2:E13 U2:W13" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F14 I2:I14 K2:K14 M2:O14 G2:G14 E2:E14 U2:W14" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7432,6 +7530,8 @@
     <hyperlink ref="D11" r:id="rId8" xr:uid="{1ED175BB-E356-4421-9580-06B490802E99}"/>
     <hyperlink ref="D12" r:id="rId9" xr:uid="{68C96D03-3D77-41F0-83D7-042AEE01849A}"/>
     <hyperlink ref="D13" r:id="rId10" xr:uid="{D563E716-EB3C-44C8-975E-C7E1BEAFAF17}"/>
+    <hyperlink ref="D6" r:id="rId11" xr:uid="{16DFA824-FE40-48B4-AB05-995F323DA12B}"/>
+    <hyperlink ref="D14" r:id="rId12" xr:uid="{7588FE92-3609-439F-BEB4-D5B0353B0092}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7439,10 +7539,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AC13"/>
+  <dimension ref="A1:AC15"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -8186,6 +8286,108 @@
       <c r="AB13" s="16"/>
       <c r="AC13" s="16"/>
     </row>
+    <row r="14" spans="1:29" s="35" customFormat="1">
+      <c r="A14" s="18">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>538</v>
+      </c>
+      <c r="C14" s="16">
+        <v>1</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="O14" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="16"/>
+      <c r="Z14" s="16"/>
+      <c r="AA14" s="16"/>
+      <c r="AB14" s="16"/>
+      <c r="AC14" s="16"/>
+    </row>
+    <row r="15" spans="1:29" s="35" customFormat="1">
+      <c r="A15" s="18">
+        <v>31</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>538</v>
+      </c>
+      <c r="C15" s="16">
+        <v>1</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="O15" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="16"/>
+      <c r="W15" s="16"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="16"/>
+      <c r="Z15" s="16"/>
+      <c r="AA15" s="16"/>
+      <c r="AB15" s="16"/>
+      <c r="AC15" s="16"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576" xr:uid="{00000000-0002-0000-0400-000000000000}">
@@ -8261,11 +8463,11 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H2" sqref="H2"/>
       <selection pane="topRight" activeCell="H2" sqref="H2"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -8892,9 +9094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
@@ -9342,7 +9542,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -9578,10 +9778,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -9883,7 +10083,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="4" customFormat="1">
+    <row r="7" spans="1:16" s="4" customFormat="1" ht="29">
       <c r="A7" s="18">
         <v>31</v>
       </c>
@@ -9893,40 +10093,44 @@
       <c r="C7" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
+      <c r="D7" s="29" t="s">
+        <v>647</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>401</v>
+      </c>
       <c r="F7" s="29" t="s">
-        <v>69</v>
+        <v>636</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>70</v>
+        <v>637</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>71</v>
+        <v>638</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>74</v>
+        <v>648</v>
       </c>
       <c r="J7" s="29" t="s">
         <v>76</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>72</v>
+        <v>639</v>
       </c>
       <c r="L7" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="M7" s="29">
-        <v>2000</v>
+        <v>640</v>
+      </c>
+      <c r="M7" s="29" t="s">
+        <v>641</v>
       </c>
       <c r="N7" s="29" t="s">
-        <v>74</v>
+        <v>642</v>
       </c>
       <c r="O7" s="30" t="s">
-        <v>75</v>
+        <v>643</v>
       </c>
       <c r="P7" s="31" t="s">
-        <v>146</v>
+        <v>644</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="4" customFormat="1">
@@ -10471,9 +10675,59 @@
         <v>146</v>
       </c>
     </row>
+    <row r="19" spans="1:16" s="33" customFormat="1">
+      <c r="A19" s="44">
+        <v>13</v>
+      </c>
+      <c r="B19" s="44" t="s">
+        <v>522</v>
+      </c>
+      <c r="C19" s="44">
+        <v>1</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>400</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>401</v>
+      </c>
+      <c r="F19" s="44" t="s">
+        <v>633</v>
+      </c>
+      <c r="G19" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="I19" s="44" t="s">
+        <v>634</v>
+      </c>
+      <c r="J19" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="K19" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="L19" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="M19" s="44" t="s">
+        <v>402</v>
+      </c>
+      <c r="N19" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="O19" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="P19" s="44" t="s">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="B10:B18">
+  <conditionalFormatting sqref="B10:B19">
     <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
@@ -10672,9 +10926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -10881,9 +11133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -11143,9 +11393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
@@ -11373,11 +11621,11 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H2" sqref="H2"/>
       <selection pane="topRight" activeCell="H2" sqref="H2"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -11622,10 +11870,10 @@
         <v>1</v>
       </c>
       <c r="D14" s="18">
-        <v>225505</v>
+        <v>225504</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>156</v>
+        <v>579</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -11843,10 +12091,10 @@
         <v>1</v>
       </c>
       <c r="D27" s="18">
-        <v>225505</v>
+        <v>225504</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>156</v>
+        <v>579</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -12107,7 +12355,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -12269,10 +12517,10 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -12512,7 +12760,7 @@
         <v>314</v>
       </c>
       <c r="J7" s="73" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -13565,7 +13813,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -13935,32 +14183,76 @@
       </c>
       <c r="L10" s="18"/>
     </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
+    <row r="11" spans="1:12" s="33" customFormat="1" ht="18" customHeight="1">
+      <c r="A11" s="18">
+        <v>13</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>515</v>
+      </c>
+      <c r="C11" s="18">
+        <v>1</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>610</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>632</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>631</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>635</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="K11" s="18">
+        <v>18</v>
+      </c>
       <c r="L11" s="18"/>
     </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
+    <row r="12" spans="1:12" s="33" customFormat="1" ht="18" customHeight="1">
+      <c r="A12" s="18">
+        <v>31</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>515</v>
+      </c>
+      <c r="C12" s="18">
+        <v>1</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>610</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>632</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>631</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>646</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="K12" s="18">
+        <v>19</v>
+      </c>
       <c r="L12" s="18"/>
     </row>
     <row r="13" spans="1:12">
@@ -13980,10 +14272,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J10" xr:uid="{00000000-0002-0000-1800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12" xr:uid="{00000000-0002-0000-1800-000000000000}">
       <formula1>"Main Website,Incredible Connection"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G10 F11:F1048576" xr:uid="{00000000-0002-0000-1800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G12 F13:F1048576" xr:uid="{00000000-0002-0000-1800-000001000000}">
       <formula1>"SAID,Passport"</formula1>
     </dataValidation>
   </dataValidations>
@@ -13997,10 +14289,12 @@
     <hyperlink ref="F8" r:id="rId7" display="TestAutomation2@gmail.com" xr:uid="{385CB16C-F360-40A0-BB9E-61E91B37FC42}"/>
     <hyperlink ref="F9" r:id="rId8" display="TestAutomation2@gmail.com" xr:uid="{DA39F455-083E-430F-AD35-9AFC0110AC38}"/>
     <hyperlink ref="F10" r:id="rId9" display="TestAutomation2@gmail.com" xr:uid="{B7395BA8-34EB-4EE0-86D9-36B1B9005493}"/>
+    <hyperlink ref="F11" r:id="rId10" display="TestAutomation2@gmail.com" xr:uid="{15DB716B-5106-4D16-807E-10D903E4E56E}"/>
+    <hyperlink ref="F12" r:id="rId11" display="TestAutomation2@gmail.com" xr:uid="{5143B6EE-B9E1-4E26-9388-C83E9574B79A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
-  <legacyDrawing r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
+  <legacyDrawing r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -15214,8 +15508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920941E8-63A8-46DF-9CEB-D9EA33709737}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -15701,13 +15995,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD40FD6A-3206-4F33-9099-D76F7461AC19}">
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T4" sqref="T4"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -16524,18 +16818,138 @@
         <v>91</v>
       </c>
     </row>
+    <row r="14" spans="1:20" ht="29">
+      <c r="A14" s="18">
+        <v>13</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>594</v>
+      </c>
+      <c r="C14" s="13">
+        <v>1</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="J14" s="13">
+        <v>2222230</v>
+      </c>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="N14" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="O14" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="P14" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q14" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="R14" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="S14" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="T14" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="29">
+      <c r="A15" s="18">
+        <v>31</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>594</v>
+      </c>
+      <c r="C15" s="13">
+        <v>1</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="J15" s="13">
+        <v>2222231</v>
+      </c>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="N15" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="O15" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="P15" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q15" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="R15" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="S15" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="T15" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M13" xr:uid="{FF70BC0E-3989-4E4A-9EDB-1D6DA4A25EBB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M15" xr:uid="{FF70BC0E-3989-4E4A-9EDB-1D6DA4A25EBB}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N13" xr:uid="{D81261F8-C548-4AA4-9D26-48EC0E008ACF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N15" xr:uid="{D81261F8-C548-4AA4-9D26-48EC0E008ACF}">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I13 P2:T13" xr:uid="{9A1E9D13-8395-4C31-BF32-7E3AFBE71119}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I15 P2:T15" xr:uid="{9A1E9D13-8395-4C31-BF32-7E3AFBE71119}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L13" xr:uid="{26B96BFD-6003-4E83-A937-3CEE292F260C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L15" xr:uid="{26B96BFD-6003-4E83-A937-3CEE292F260C}">
       <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
     </dataValidation>
   </dataValidations>
@@ -16609,10 +17023,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E7D9075-5F21-450D-8059-BA8C0176E98B}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -16693,30 +17107,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="40">
+        <v>31</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>581</v>
+      </c>
+      <c r="C7" s="40">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16865,32 +17272,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16907,4 +17307,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>